<commit_message>
Add button to panel in "answer template" doc
</commit_message>
<xml_diff>
--- a/answer template.xlsx
+++ b/answer template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miriam.romero\Documents\macro-excel\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miriam.romero\Documents\macro-excel\vbaTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB8DE0E-F0B1-4759-90B3-556FA5B0598D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52581AC0-0EAA-4545-A2EA-2B3639CB0D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Panel" sheetId="1" r:id="rId1"/>
+    <sheet name="Panel" sheetId="3" r:id="rId1"/>
     <sheet name="answer template" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="268">
   <si>
     <t>Advanced</t>
   </si>
@@ -844,9 +844,6 @@
   </si>
   <si>
     <t>Question</t>
-  </si>
-  <si>
-    <t>Introduce el id</t>
   </si>
 </sst>
 </file>
@@ -868,18 +865,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -920,7 +911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -931,7 +922,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,6 +937,84 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>457200</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3073" name="Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3073"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000010C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="36576" bIns="32004" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Iniciar script</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1211,29 +1279,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C93F75D-2A56-4B0B-B6F6-799DC0ECC827}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="C3:E4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="E4" s="4"/>
-    </row>
-  </sheetData>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3073" r:id="rId3" name="Button 1">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!ThisWorkbook.GenerarInformeConID">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>571500</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>85725</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>457200</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>85725</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -1242,9 +1328,9 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A5:F246"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>